<commit_message>
REV commit: 3 AUG 11.17 AM
</commit_message>
<xml_diff>
--- a/uploads/input.xlsx
+++ b/uploads/input.xlsx
@@ -851,8 +851,8 @@
   </sheetPr>
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
-        <f>A45</f>
+        <f>A46</f>
         <v>12</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -920,7 +920,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <f>IF(Sheet3!B2+2&gt;(A32-2),A32-5,Sheet3!B2+2)</f>
+        <f>IF(Sheet3!B2+2&gt;(A33-2),A33-5,Sheet3!B2+2)</f>
         <v>100</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -1137,8 +1137,8 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
-        <f>A24+(A29*A47)</f>
-        <v>43.2</v>
+        <f>A24+(A29*A30)</f>
+        <v>388.8</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>79</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>83</v>
@@ -1192,60 +1192,60 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="10">
+        <v>10.8</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
         <f>A25-A24</f>
-        <v>43.2</v>
-      </c>
-      <c r="B30" s="13" t="s">
+        <v>388.8</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C31" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <v>0</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B32" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <f>A23</f>
         <v>110.97499999999999</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>110</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
-        <v>0.22500000000000001</v>
+        <v>110</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1253,43 +1253,43 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>11.1</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>0.9</v>
+        <v>11.1</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1297,43 +1297,43 @@
         <v>0.75</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
-        <v>110</v>
+        <v>0.75</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
-        <v>109.4</v>
+        <v>110</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
-        <v>1.2</v>
+        <v>109.4</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,54 +1341,54 @@
         <v>1.2</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C44" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
         <v>10</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C45" s="15" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
-        <v>12</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
-        <v>10.8</v>
+        <v>1</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
REV commit: 3 AUG 13.00 HOURS
</commit_message>
<xml_diff>
--- a/uploads/input.xlsx
+++ b/uploads/input.xlsx
@@ -190,12 +190,6 @@
     <t>Read Chainage Of Left Abutment TO BE INCRESED FOR COMPLETE DRAWING OF APPROACH</t>
   </si>
   <si>
-    <t>Abt Left Front Batter ( 1 HOR : 10 VER &gt;&gt;&gt;&gt;&gt; VALUE 10)</t>
-  </si>
-  <si>
-    <t>Abt Left  Toe Batter ( 1 HOR : 5 VER &gt;&gt;&gt;&gt;&gt; VALUE 5)</t>
-  </si>
-  <si>
     <t>Abutment RIGHT Footing Level</t>
   </si>
   <si>
@@ -377,6 +371,12 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Abt Left Front Batter ( e.g. 1 HOR : 10 VER &gt;&gt;&gt;&gt;&gt; VALUE 10)</t>
+  </si>
+  <si>
+    <t>Abt Left  Toe Batter (e.g.  1 HOR : 5 VER &gt;&gt;&gt;&gt;&gt; VALUE 5)</t>
   </si>
 </sst>
 </file>
@@ -851,8 +851,8 @@
   </sheetPr>
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,354 +864,354 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="19">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <f>A2+(A5*A6)</f>
+        <v>388.8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>36</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>10.8</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <f>A3-A2</f>
+        <v>388.8</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>186</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="B8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <f>A46</f>
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <f>IF(Sheet3!B2+2&gt;(A33-2),A33-5,Sheet3!B2+2)</f>
         <v>100</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="B12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <f>A6+0.75</f>
-        <v>100.75</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>1.2</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>10</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <f>A6+A16</f>
-        <v>101</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <f>A7</f>
-        <v>100.75</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
-        <f>A6+A16</f>
-        <v>101</v>
+        <f>A12+0.75</f>
+        <v>100.75</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <f>A11</f>
-        <v>100.75</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>55</v>
+      <c r="A14" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>1</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>34</v>
+      <c r="A16" s="12">
+        <f>A12+A22</f>
+        <v>101</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <v>3</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>35</v>
+      <c r="A17" s="12">
+        <f>A13</f>
+        <v>100.75</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <f>A10</f>
-        <v>101</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>107</v>
+      <c r="A18" s="10">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <f>A11</f>
+        <f>A12+A22</f>
+        <v>101</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <f>A17</f>
         <v>100.75</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>100</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>36</v>
+      <c r="B20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
-        <v>0</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>3</v>
+      <c r="A21" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
+        <v>1</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>3</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <f>A16</f>
+        <v>101</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <f>A17</f>
+        <v>100.75</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>100</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <v>0</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>100</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <v>110.97499999999999</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
-        <v>0</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <f>A24+(A29*A30)</f>
-        <v>388.8</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>10</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
-        <v>21</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
-        <v>36</v>
-      </c>
       <c r="B29" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>10.8</v>
+        <v>10</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
-        <f>A25-A24</f>
-        <v>388.8</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>38</v>
+      <c r="A31" s="10">
+        <v>1</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>50</v>
@@ -1227,11 +1227,11 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <f>A23</f>
+        <f>A29</f>
         <v>110.97499999999999</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>39</v>
@@ -1242,7 +1242,7 @@
         <v>110</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>9</v>
@@ -1253,7 +1253,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>10</v>
@@ -1264,7 +1264,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>40</v>
@@ -1275,7 +1275,7 @@
         <v>11.1</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>41</v>
@@ -1286,7 +1286,7 @@
         <v>0.9</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>42</v>
@@ -1297,7 +1297,7 @@
         <v>0.75</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>43</v>
@@ -1308,7 +1308,7 @@
         <v>0.75</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>44</v>
@@ -1319,10 +1319,10 @@
         <v>110</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,10 +1330,10 @@
         <v>109.4</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>1.2</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>45</v>
@@ -1352,7 +1352,7 @@
         <v>1.2</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>11</v>
@@ -1363,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>12</v>
@@ -1374,7 +1374,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>13</v>
@@ -1385,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>46</v>
@@ -1440,7 +1440,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>27</v>
@@ -1451,7 +1451,7 @@
         <v>3.5</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>31</v>
@@ -1463,7 +1463,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>28</v>
@@ -1474,7 +1474,7 @@
         <v>0.375</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>29</v>
@@ -1485,7 +1485,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>30</v>

</xml_diff>